<commit_message>
aspiration example set up (only trainer missing)
</commit_message>
<xml_diff>
--- a/examples/Aspiration/data/excel_source/scenarios.xlsx
+++ b/examples/Aspiration/data/excel_source/scenarios.xlsx
@@ -384,7 +384,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +462,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -512,7 +512,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>100</v>

</xml_diff>